<commit_message>
update script for excel files
</commit_message>
<xml_diff>
--- a/data_templates/FMECA_Sample.xlsx
+++ b/data_templates/FMECA_Sample.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loictiemani/Desktop/MasterDataGovernance/Untitled/Master-Data-Governance-SAP/data_templates/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6D4C41-B84A-B246-80A7-803588318839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="78900" yWindow="2340" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -379,8 +373,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,21 +437,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -495,7 +481,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -529,7 +515,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -564,10 +549,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -740,24 +724,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,7 +751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -797,7 +771,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -817,7 +791,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -837,7 +811,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -857,7 +831,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -877,7 +851,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -897,7 +871,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -917,7 +891,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -937,7 +911,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -957,7 +931,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -977,7 +951,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -997,7 +971,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1017,7 +991,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1037,7 +1011,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1057,7 +1031,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1077,7 +1051,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1097,7 +1071,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1117,7 +1091,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1137,7 +1111,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1157,7 +1131,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1177,7 +1151,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1197,7 +1171,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1217,7 +1191,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1237,7 +1211,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1257,7 +1231,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1277,7 +1251,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1297,7 +1271,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1317,7 +1291,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1337,7 +1311,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1357,7 +1331,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1377,7 +1351,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1397,7 +1371,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1417,7 +1391,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1437,7 +1411,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1457,7 +1431,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1477,7 +1451,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1497,7 +1471,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1517,7 +1491,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1537,7 +1511,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -1557,7 +1531,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1577,7 +1551,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1597,7 +1571,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -1617,7 +1591,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1637,7 +1611,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1657,7 +1631,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -1677,7 +1651,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -1697,7 +1671,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1717,7 +1691,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1737,7 +1711,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1757,7 +1731,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>55</v>
       </c>

</xml_diff>